<commit_message>
refactor: Update A* algorithm and settings handling in A_Star_Implementation.py
</commit_message>
<xml_diff>
--- a/execution_times.xlsx
+++ b/execution_times.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\3zoza\Desktop\Code\Python Workspace\AStar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0B5106-65F1-4DF5-8BF3-7A9416DF7BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796D75CB-C791-4065-A931-0CCAFF292EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{159DDC5E-64DC-4355-8E75-8E73F8EC1159}"/>
   </bookViews>
@@ -967,7 +967,7 @@
   <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>